<commit_message>
let testurl can read test_host and test_port from APITestCase.xlsx,url did`t write like "http://XXX.XXX.XXX.XXX:XXXX/X/X",only write "/X/X/"
</commit_message>
<xml_diff>
--- a/data/APITestCase.xlsx
+++ b/data/APITestCase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\systemdocument\桌面\study\code\ApiAutoTest\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\systemdocument\桌面\work\测试脚本\接口测试脚本\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEB4C5B-2A22-4605-A7D1-97757C5DAAA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9430B6A6-7540-43EC-AB3E-5C3DF86E7D3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>event_query_001</t>
   </si>
@@ -82,38 +82,69 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>尝试登录云村</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"Content-Type":"application/json;charset=UTF-8"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"username":"18758198021","password":"TTFGUVIzbHVOMGhxTWpKUmJuaE5iWG95WkRZNE4wRTNXbWxDU21SSVMxcEFjMmxvWVdsNWFXTjFia0I1ZURKSGFtTTRNME5RTTA0NFUyWTRPSEF5V0dadVRYSlJOMWhvUzBGNVJnPT0=","platform":"OPERATION"}</t>
+  </si>
+  <si>
+    <t>json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>code</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>3001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>用户不存在！</t>
   </si>
   <si>
-    <t>登录</t>
-  </si>
-  <si>
-    <t>登录后台测试</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:3002/login</t>
-  </si>
-  <si>
-    <t>post</t>
-  </si>
-  <si>
-    <t>{"Content-Type":"application/json;charset=UTF-8"}</t>
-  </si>
-  <si>
-    <t>{"username":"18758198021","password":"TTFGUVIMxcEFjMmxvWVdsNWFXTjFia0I1ZURKSGFtTTRNME5RTTA0NFUyWTRPSEF5V0dadVRYSlJOMWhvUzBGNVJnPT0=","platform":"OPERATION"}</t>
+    <t>登录云村后台测试失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录云村后台测试成功</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"username":"18758198024","password":"TTFGUVIzbHVOMGhxTWpKUmJuaE5iWG95WkRZNE4wRTNXbWxDU21SSVMxcEFjMmxvWVdsNWFXTjFia0I1ZURKSGFtTTRNME5RTTA0NFUyWTRPSEF5V0dadVRYSlJOMWhvUzBGNVJnPT0=","platform":"OPERATION"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>200</t>
-  </si>
-  <si>
-    <t>3001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>success</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>event_query_002</t>
+  </si>
+  <si>
+    <t>/sso/cloudUser/login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -599,17 +630,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:M3"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="36.21875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.21875" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="11" style="3" customWidth="1"/>
@@ -652,7 +683,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>10</v>
@@ -666,55 +697,77 @@
     </row>
     <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="11">
+        <v>200</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="L2" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="M2" s="7"/>
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="M3" s="6"/>
       <c r="N3" s="5"/>
     </row>

</xml_diff>